<commit_message>
Add client love as per Seth's request
</commit_message>
<xml_diff>
--- a/Templates/03-employee-review-kpis.xlsx
+++ b/Templates/03-employee-review-kpis.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SSW.EmployeeKPIs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SSW.EmployeeKPIs\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{287BD6CB-3B4D-4D3E-BBAC-10FF486C3DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41802C64-34E2-4C7A-8C4A-9B45175F2FB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5400" yWindow="0" windowWidth="16200" windowHeight="9307" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Annual Review KPIs - {{ EMPLOYEE NAME }}</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>⭐ Checked by {{ EMPLOYEE NAME }}</t>
+  </si>
+  <si>
+    <t>Client love</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F8" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -942,39 +945,44 @@
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A21" s="7" t="s">
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5">
+        <f>PRODUCT(C21:D21) * 10</f>
+        <v>2</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A22" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="8">
-        <f>SUM(E3:E20)</f>
-        <v>82</v>
-      </c>
-      <c r="F21" s="9">
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="8">
+        <f>SUM(E3:E21)</f>
+        <v>84</v>
+      </c>
+      <c r="F22" s="9">
         <f>SUM(C3:C20) * 100</f>
         <v>820.00000000000011</v>
       </c>
-      <c r="G21" s="10">
-        <f xml:space="preserve"> E21/F21</f>
-        <v>9.9999999999999992E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="4" t="s">
-        <v>38</v>
-      </c>
+      <c r="G22" s="10">
+        <f xml:space="preserve"> E22/F22</f>
+        <v>0.10243902439024388</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
+      <c r="A23" s="6"/>
       <c r="B23" s="6"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -982,34 +990,23 @@
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
     </row>
+    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="212980c9-5617-46ce-99ad-a376bd4152d0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文档" ma:contentTypeID="0x010100EF9B896C278B3E4A966930FF26B3A803" ma:contentTypeVersion="17" ma:contentTypeDescription="新建文档。" ma:contentTypeScope="" ma:versionID="d1d78c8ee01d152b02ca9ec89016707f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="212980c9-5617-46ce-99ad-a376bd4152d0" xmlns:ns3="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae87d36dae376fc2439eed63ad162587" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -1257,27 +1254,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B17A44F8-5891-455F-A1D4-2DD47FB28B38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="212980c9-5617-46ce-99ad-a376bd4152d0"/>
-    <ds:schemaRef ds:uri="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CABC0E4-6C66-4C9C-9C06-5E7EF7DC0FA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="212980c9-5617-46ce-99ad-a376bd4152d0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{224F5FEA-A32B-444E-904D-0AF18D5B10B9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1295,4 +1294,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CABC0E4-6C66-4C9C-9C06-5E7EF7DC0FA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B17A44F8-5891-455F-A1D4-2DD47FB28B38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="212980c9-5617-46ce-99ad-a376bd4152d0"/>
+    <ds:schemaRef ds:uri="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated styling for spreadsheet
Based on email chain: URGENT 🚨 Do you have KPIs for your Annual Employee Reviews? | SSW.Rules
</commit_message>
<xml_diff>
--- a/Templates/03-employee-review-kpis.xlsx
+++ b/Templates/03-employee-review-kpis.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\SSW.EmployeeKPIs\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bettybondoc/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5181D5E-11B5-4C17-881B-F46AB031AA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151982F2-2BAE-B64B-922D-326869520F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="280" yWindow="500" windowWidth="30720" windowHeight="17720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="3" r:id="rId1"/>
+    <sheet name="Sample (Bob)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="64">
   <si>
     <t>Annual Review KPIs - {{ EMPLOYEE NAME }}</t>
   </si>
@@ -149,12 +150,6 @@
     <t>Inbox count</t>
   </si>
   <si>
-    <t>Overall</t>
-  </si>
-  <si>
-    <t>⭐ Checked by {{ EMPLOYEE NAME }}</t>
-  </si>
-  <si>
     <t>Client love</t>
   </si>
   <si>
@@ -162,13 +157,85 @@
   </si>
   <si>
     <t>e.g. Adam</t>
+  </si>
+  <si>
+    <t>Annual Review KPIs - Bob Northwind</t>
+  </si>
+  <si>
+    <t>OVERALL</t>
+  </si>
+  <si>
+    <t>⭐</t>
+  </si>
+  <si>
+    <t>Checked by Bob Northwind</t>
+  </si>
+  <si>
+    <t>💼</t>
+  </si>
+  <si>
+    <t>😊</t>
+  </si>
+  <si>
+    <t>👫</t>
+  </si>
+  <si>
+    <t>👀</t>
+  </si>
+  <si>
+    <t>🏆</t>
+  </si>
+  <si>
+    <t>🔍</t>
+  </si>
+  <si>
+    <t>🤝</t>
+  </si>
+  <si>
+    <t>📝</t>
+  </si>
+  <si>
+    <t>🎥</t>
+  </si>
+  <si>
+    <t>🌐</t>
+  </si>
+  <si>
+    <t>🏃</t>
+  </si>
+  <si>
+    <t>📥</t>
+  </si>
+  <si>
+    <t>❤️</t>
+  </si>
+  <si>
+    <t>🧑‍💼</t>
+  </si>
+  <si>
+    <t>🎓</t>
+  </si>
+  <si>
+    <t>🙌</t>
+  </si>
+  <si>
+    <t>📖</t>
+  </si>
+  <si>
+    <t>📜</t>
+  </si>
+  <si>
+    <t>🔢</t>
+  </si>
+  <si>
+    <t>Checked by {{ EMPLOYEE NAME }}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -177,42 +244,117 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
       <sz val="28"/>
-      <color rgb="FF000000"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="HelveticaNeueLTStd-Bd"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="28"/>
+      <color theme="1" tint="0.249977111117893"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Aptos"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
+      <name val="Aptos"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
+      <b/>
+      <sz val="28"/>
+      <color theme="1" tint="0.249977111117893"/>
       <name val="Aptos"/>
-      <family val="2"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Aptos"/>
-      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="HelveticaNeueLTStd-Roman"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,18 +363,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -240,38 +400,312 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="2"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="19" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFDE303A"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -599,428 +1033,1665 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C8163E-F78A-3442-870F-8E03F85460B1}">
+  <dimension ref="A1:S28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.265625" customWidth="1"/>
-    <col min="2" max="2" width="10.1328125" customWidth="1"/>
-    <col min="3" max="3" width="7.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1328125" customWidth="1"/>
-    <col min="5" max="5" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="0.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="36.4" x14ac:dyDescent="0.85">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+    </row>
+    <row r="2" spans="1:19" ht="47" customHeight="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="23" customHeight="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C3" s="46"/>
+      <c r="D3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="F3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="G3" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="H3" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I3" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J3" s="49" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" ht="23" customHeight="1">
+      <c r="A4" s="30"/>
+      <c r="B4" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4">
+      <c r="D4" s="51"/>
+      <c r="E4" s="52">
         <v>1</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="5">
-        <f>PRODUCT(C3:D3) * 10</f>
+      <c r="F4" s="52"/>
+      <c r="G4" s="53">
+        <f>PRODUCT(E4:F4) * 10</f>
         <v>10</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="H4" s="54"/>
+      <c r="I4" s="54"/>
+      <c r="J4" s="55"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="23" customHeight="1">
+      <c r="A5" s="30"/>
+      <c r="B5" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4">
+      <c r="D5" s="51"/>
+      <c r="E5" s="52">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="5">
-        <f t="shared" ref="E4:E19" si="0">PRODUCT(C4:D4) * 10</f>
+      <c r="F5" s="52"/>
+      <c r="G5" s="53">
+        <f t="shared" ref="G5:G20" si="0">PRODUCT(E5:F5) * 10</f>
         <v>10</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+      <c r="H5" s="54"/>
+      <c r="I5" s="54"/>
+      <c r="J5" s="55"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" ht="23" customHeight="1">
+      <c r="A6" s="30"/>
+      <c r="B6" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4">
+      <c r="D6" s="51"/>
+      <c r="E6" s="52">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="5">
+      <c r="F6" s="52"/>
+      <c r="G6" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
+      <c r="H6" s="54"/>
+      <c r="I6" s="54"/>
+      <c r="J6" s="55"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="46" customHeight="1">
+      <c r="A7" s="30"/>
+      <c r="B7" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4">
+      <c r="D7" s="51"/>
+      <c r="E7" s="52">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5">
+      <c r="F7" s="52"/>
+      <c r="G7" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="H7" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="6"/>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+      <c r="I7" s="54"/>
+      <c r="J7" s="55"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="23" customHeight="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4">
+      <c r="D8" s="51"/>
+      <c r="E8" s="52">
         <v>1</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="5">
+      <c r="F8" s="52"/>
+      <c r="G8" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
+      <c r="H8" s="54"/>
+      <c r="I8" s="54"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" ht="23" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4">
+      <c r="D9" s="51"/>
+      <c r="E9" s="52">
         <v>1</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="5">
+      <c r="F9" s="52"/>
+      <c r="G9" s="53">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
+      <c r="H9" s="54"/>
+      <c r="I9" s="54"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="4" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="57"/>
+      <c r="D10" s="58"/>
+      <c r="E10" s="58"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="60"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" ht="23" customHeight="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="50" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4">
+      <c r="D11" s="52"/>
+      <c r="E11" s="52">
         <v>0.25</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="5">
+      <c r="F11" s="52"/>
+      <c r="G11" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="H11" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
+      <c r="I11" s="54"/>
+      <c r="J11" s="55"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" ht="23" customHeight="1">
+      <c r="A12" s="30"/>
+      <c r="B12" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4">
+      <c r="D12" s="52"/>
+      <c r="E12" s="52">
         <v>0.25</v>
       </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="5">
+      <c r="F12" s="52"/>
+      <c r="G12" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="H12" s="54" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="6"/>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A12" s="4" t="s">
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="23" customHeight="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="50" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4">
+      <c r="D13" s="52"/>
+      <c r="E13" s="52">
         <v>0.25</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="5">
+      <c r="F13" s="52"/>
+      <c r="G13" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="H13" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A13" s="4" t="s">
+      <c r="I13" s="54"/>
+      <c r="J13" s="55"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="23" customHeight="1">
+      <c r="A14" s="30"/>
+      <c r="B14" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4">
+      <c r="D14" s="52"/>
+      <c r="E14" s="52">
         <v>0.25</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="5">
+      <c r="F14" s="52"/>
+      <c r="G14" s="53">
+        <f>PRODUCT(E14:F14) * 10</f>
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="54" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="54"/>
+      <c r="J14" s="55"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="23" customHeight="1">
+      <c r="A15" s="30"/>
+      <c r="B15" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52">
+        <v>0.25</v>
+      </c>
+      <c r="F15" s="52"/>
+      <c r="G15" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13" s="6"/>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4">
+      <c r="H15" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="54"/>
+      <c r="J15" s="55"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="23" customHeight="1">
+      <c r="A16" s="30"/>
+      <c r="B16" s="63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52">
         <v>0.25</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="5">
+      <c r="F16" s="52"/>
+      <c r="G16" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G14" s="6"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4">
+      <c r="H16" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="54"/>
+      <c r="J16" s="55"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="23" customHeight="1">
+      <c r="A17" s="30"/>
+      <c r="B17" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52">
         <v>0.25</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="5">
+      <c r="F17" s="52"/>
+      <c r="G17" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A16" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4">
+      <c r="H17" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="54"/>
+      <c r="J17" s="55"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" ht="23" customHeight="1">
+      <c r="A18" s="30"/>
+      <c r="B18" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="64" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52">
         <v>0.25</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="5">
+      <c r="F18" s="52"/>
+      <c r="G18" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="6"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4">
+      <c r="H18" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" ht="23" customHeight="1">
+      <c r="A19" s="30"/>
+      <c r="B19" s="50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52">
         <v>0.25</v>
       </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="5">
+      <c r="F19" s="52"/>
+      <c r="G19" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="6"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4">
+      <c r="H19" s="54" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" s="54"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" ht="23" customHeight="1">
+      <c r="A20" s="30"/>
+      <c r="B20" s="63" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="64" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52">
         <v>0.25</v>
       </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="5">
+      <c r="F20" s="52"/>
+      <c r="G20" s="53">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="H20" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="54"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" ht="23" customHeight="1">
+      <c r="A21" s="30"/>
+      <c r="B21" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52">
+        <v>0.25</v>
+      </c>
+      <c r="F21" s="52"/>
+      <c r="G21" s="53">
+        <f>PRODUCT(E21:F21) * 10</f>
+        <v>2.5</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="54"/>
+      <c r="J21" s="55"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" ht="23" customHeight="1">
+      <c r="A22" s="30"/>
+      <c r="B22" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52">
+        <v>0.25</v>
+      </c>
+      <c r="F22" s="52"/>
+      <c r="G22" s="53">
+        <f>PRODUCT(E22:F22) * 10</f>
+        <v>2.5</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" ht="23" hidden="1" customHeight="1">
+      <c r="A23" s="30"/>
+      <c r="B23" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="79" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="74">
+        <f>SUM(G4:G22)</f>
+        <v>90</v>
+      </c>
+      <c r="H23" s="75">
+        <f>SUM(E4:E21) * 100</f>
+        <v>875</v>
+      </c>
+      <c r="I23" s="76">
+        <f xml:space="preserve"> G23/H23</f>
+        <v>0.10285714285714286</v>
+      </c>
+      <c r="J23" s="77"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1">
+      <c r="A24" s="30"/>
+      <c r="B24" s="67"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:19" ht="23" customHeight="1">
+      <c r="A25" s="30"/>
+      <c r="B25" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19" ht="18" customHeight="1">
+      <c r="A26" s="15"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13BCA3CA-E641-0549-9AAF-FBCA4F44DEC2}">
+  <dimension ref="A1:S28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="0.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
+    <col min="4" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="42.1640625" customWidth="1"/>
+    <col min="9" max="9" width="15.1640625" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+    </row>
+    <row r="2" spans="1:19" ht="47" customHeight="1">
+      <c r="A2" s="15"/>
+      <c r="B2" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+    </row>
+    <row r="3" spans="1:19" ht="23" customHeight="1">
+      <c r="A3" s="15"/>
+      <c r="B3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="32"/>
+      <c r="D3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" ht="23" customHeight="1">
+      <c r="A4" s="30"/>
+      <c r="B4" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="18">
+        <v>1</v>
+      </c>
+      <c r="F4" s="18">
+        <v>7</v>
+      </c>
+      <c r="G4" s="23">
+        <f>PRODUCT(E4:F4) * 10</f>
+        <v>70</v>
+      </c>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="23" customHeight="1">
+      <c r="A5" s="30"/>
+      <c r="B5" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="18">
+        <v>1</v>
+      </c>
+      <c r="F5" s="18">
+        <v>8</v>
+      </c>
+      <c r="G5" s="23">
+        <f t="shared" ref="G5:G20" si="0">PRODUCT(E5:F5) * 10</f>
+        <v>80</v>
+      </c>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" ht="23" customHeight="1">
+      <c r="A6" s="30"/>
+      <c r="B6" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="18">
+        <v>1</v>
+      </c>
+      <c r="F6" s="18">
+        <v>6</v>
+      </c>
+      <c r="G6" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="46" customHeight="1">
+      <c r="A7" s="30"/>
+      <c r="B7" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="18">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18">
+        <v>8</v>
+      </c>
+      <c r="G7" s="23">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="19"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="23" customHeight="1">
+      <c r="A8" s="30"/>
+      <c r="B8" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="18">
+        <v>1</v>
+      </c>
+      <c r="F8" s="18">
+        <v>7</v>
+      </c>
+      <c r="G8" s="23">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" ht="23" customHeight="1">
+      <c r="A9" s="30"/>
+      <c r="B9" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="18">
+        <v>1</v>
+      </c>
+      <c r="F9" s="18">
+        <v>6</v>
+      </c>
+      <c r="G9" s="23">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="4" customHeight="1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="43"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" ht="23" customHeight="1">
+      <c r="A11" s="30"/>
+      <c r="B11" s="35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F11" s="18">
+        <v>7</v>
+      </c>
+      <c r="G11" s="23">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="H11" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="19"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" ht="23" customHeight="1">
+      <c r="A12" s="30"/>
+      <c r="B12" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F12" s="18">
+        <v>7</v>
+      </c>
+      <c r="G12" s="23">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="H12" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="20"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="23" customHeight="1">
+      <c r="A13" s="30"/>
+      <c r="B13" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F13" s="18">
+        <v>3</v>
+      </c>
+      <c r="G13" s="23">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H13" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="19"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="23" customHeight="1">
+      <c r="A14" s="30"/>
+      <c r="B14" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F14" s="18">
+        <v>5</v>
+      </c>
+      <c r="G14" s="23">
+        <f t="shared" si="0"/>
+        <v>12.5</v>
+      </c>
+      <c r="H14" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14" s="19"/>
+      <c r="J14" s="20"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="23" customHeight="1">
+      <c r="A15" s="30"/>
+      <c r="B15" s="37" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F15" s="18">
+        <v>7</v>
+      </c>
+      <c r="G15" s="23">
+        <f t="shared" si="0"/>
+        <v>17.5</v>
+      </c>
+      <c r="H15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="19"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="23" customHeight="1">
+      <c r="A16" s="30"/>
+      <c r="B16" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F16" s="18">
+        <v>3</v>
+      </c>
+      <c r="G16" s="23">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="23" customHeight="1">
+      <c r="A17" s="30"/>
+      <c r="B17" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F17" s="18">
+        <v>3</v>
+      </c>
+      <c r="G17" s="23">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H17" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="20"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" ht="23" customHeight="1">
+      <c r="A18" s="30"/>
+      <c r="B18" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="18">
+        <v>10</v>
+      </c>
+      <c r="G18" s="23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="8"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" ht="23" customHeight="1">
+      <c r="A19" s="30"/>
+      <c r="B19" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F19" s="18">
+        <v>3</v>
+      </c>
+      <c r="G19" s="23">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="H19" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="G18" s="6"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A19" s="4" t="s">
+      <c r="I19" s="19"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" ht="23" customHeight="1">
+      <c r="A20" s="30"/>
+      <c r="B20" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4">
+      <c r="D20" s="18"/>
+      <c r="E20" s="18">
         <v>0.25</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="5">
+      <c r="F20" s="18">
+        <v>9</v>
+      </c>
+      <c r="G20" s="23">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-      <c r="F19" s="6" t="s">
+        <v>22.5</v>
+      </c>
+      <c r="H20" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A20" s="4" t="s">
+      <c r="I20" s="19"/>
+      <c r="J20" s="20"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" ht="23" customHeight="1">
+      <c r="A21" s="30"/>
+      <c r="B21" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4">
+      <c r="D21" s="18"/>
+      <c r="E21" s="18">
         <v>0.25</v>
       </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="5">
-        <f>PRODUCT(C20:D20) * 10</f>
-        <v>2.5</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="G20" s="6"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.45">
-      <c r="A21" s="4" t="s">
+      <c r="F21" s="18">
+        <v>8</v>
+      </c>
+      <c r="G21" s="23">
+        <f>PRODUCT(E21:F21) * 10</f>
+        <v>20</v>
+      </c>
+      <c r="H21" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" ht="23" customHeight="1">
+      <c r="A22" s="30"/>
+      <c r="B22" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="18"/>
+      <c r="E22" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="F22" s="18">
+        <v>6</v>
+      </c>
+      <c r="G22" s="23">
+        <f>PRODUCT(E22:F22) * 10</f>
+        <v>15</v>
+      </c>
+      <c r="H22" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="D21" s="4"/>
-      <c r="E21" s="5">
-        <f>PRODUCT(C21:D21) * 10</f>
-        <v>2.5</v>
-      </c>
-      <c r="F21" s="6" t="s">
+      <c r="I22" s="19"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="8"/>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+    </row>
+    <row r="23" spans="1:19" ht="23" hidden="1" customHeight="1">
+      <c r="A23" s="30"/>
+      <c r="B23" s="78" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="80" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="6"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A22" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="8">
-        <f>SUM(E3:E21)</f>
-        <v>90</v>
-      </c>
-      <c r="F22" s="9">
-        <f>SUM(C3:C20) * 100</f>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="3">
+        <f>SUM(G4:G22)</f>
+        <v>597.5</v>
+      </c>
+      <c r="H23" s="5">
+        <f>SUM(E4:E21) * 100</f>
         <v>875</v>
       </c>
-      <c r="G22" s="10">
-        <f xml:space="preserve"> E22/F22</f>
-        <v>0.10285714285714286</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="14.65" x14ac:dyDescent="0.45">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-    </row>
-    <row r="24" spans="1:7" ht="31.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
+      <c r="I23" s="6">
+        <f xml:space="preserve"> G23/H23</f>
+        <v>0.68285714285714283</v>
+      </c>
+      <c r="J23" s="22"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="10"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="8"/>
+      <c r="R23" s="8"/>
+      <c r="S23" s="8"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1">
+      <c r="A24" s="30"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="8"/>
+      <c r="R24" s="8"/>
+      <c r="S24" s="8"/>
+    </row>
+    <row r="25" spans="1:19" ht="23" customHeight="1">
+      <c r="A25" s="30"/>
+      <c r="B25" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="8"/>
+      <c r="R25" s="8"/>
+      <c r="S25" s="8"/>
+    </row>
+    <row r="26" spans="1:19" ht="18" customHeight="1">
+      <c r="A26" s="15"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+    </row>
+    <row r="27" spans="1:19">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+    </row>
+    <row r="28" spans="1:19">
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -1031,15 +2702,6 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1291,6 +2953,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CABC0E4-6C66-4C9C-9C06-5E7EF7DC0FA2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B17A44F8-5891-455F-A1D4-2DD47FB28B38}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1298,14 +2968,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="212980c9-5617-46ce-99ad-a376bd4152d0"/>
     <ds:schemaRef ds:uri="0ecd88e7-26cc-4a6b-8b5c-6a9962e64f6a"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9CABC0E4-6C66-4C9C-9C06-5E7EF7DC0FA2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>